<commit_message>
Updated Analise Financeira Projeto 1
</commit_message>
<xml_diff>
--- a/Analise Financeira/Análise Financeira PROJ1.xlsx
+++ b/Analise Financeira/Análise Financeira PROJ1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gestao-de-Portfolios\Analise Financeira\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64F56D2-496D-4658-A85E-65D7EBF31A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32072C6-A334-4A72-A65A-DA9150BDD14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showSheetTabs="0" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{5407E0C7-D3D1-4456-BA1C-167F3E5756A9}"/>
   </bookViews>
@@ -193,7 +193,7 @@
     <t>PROJETO:</t>
   </si>
   <si>
-    <t>Com uma Taxa Mínima de Atratividade (TMA) de 10%, o projeto mostra-se financeiramente viável. O Valor Presente Líquido (VPL) é positivo, alcançando R$ 331.969,87, indicando que o projeto gera mais valor do que o custo inicial de R$ 1.584.000,00. O período de payback, ou seja, o tempo necessário para recuperar o investimento inicial, é de aproximadamente 6 anos. O Retorno sobre o Investimento (ROI) é de 77%, destacando a atratividade financeira do projeto. Portanto, é recomendada a sua aprovação, pois apresenta um retorno significativo com uma relação de risco satisfatória.</t>
+    <t>Com uma Taxa Mínima de Atratividade (TMA) de 11%, o projeto continua sendo financeiramente viável. O Valor Presente Líquido (VPL) é positivo, atingindo R$ 266.545,94, o que indica que o valor presente dos fluxos de caixa futuros supera o investimento inicial de R$ 1.584.000,00. O período de payback é de aproximadamente 5,29 anos, destacando um tempo relativamente longo para recuperar o capital investido. A Taxa Interna de Retorno (TIR) de 15,68% supera a TMA de 11%, sugerindo que o projeto oferece um retorno superior ao custo de oportunidade do capital. Com um Retorno sobre o Investimento (ROI) de 77%, o projeto demonstra uma boa relação custo-benefício e reforça sua atratividade financeira. Portanto, é recomendada sua aprovação, pois o projeto oferece um retorno significativo com risco controlado.</t>
   </si>
 </sst>
 </file>
@@ -3230,8 +3230,8 @@
   <dimension ref="B2:G25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14:G19"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3322,17 +3322,17 @@
       </c>
       <c r="D8" s="13">
         <f t="shared" ref="D8:D19" si="0">PV($G$8,B8,,-C8)</f>
-        <v>227272.72727272726</v>
+        <v>225225.22522522521</v>
       </c>
       <c r="E8" s="13">
         <f>D8+E7</f>
-        <v>-1356727.2727272727</v>
+        <v>-1358774.7747747749</v>
       </c>
       <c r="F8" s="25" t="s">
         <v>10</v>
       </c>
       <c r="G8" s="18">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3344,18 +3344,18 @@
       </c>
       <c r="D9" s="13">
         <f t="shared" si="0"/>
-        <v>247933.88429752062</v>
+        <v>243486.72997321642</v>
       </c>
       <c r="E9" s="13">
         <f t="shared" ref="E9:E19" si="1">D9+E8</f>
-        <v>-1108793.3884297521</v>
+        <v>-1115288.0448015584</v>
       </c>
       <c r="F9" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G9" s="15">
         <f>IF(G11&lt;0,"PROJETO INVIÁVEL",MATCH(0,E7:E19,1)-1+(-INDEX(E7:E19,MATCH(0,E7:E19,1))/INDEX(D7:D19,MATCH(0,E7:E19,1)+1)))</f>
-        <v>5.1598501771428582</v>
+        <v>5.2877836983543212</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3367,11 +3367,11 @@
       </c>
       <c r="D10" s="13">
         <f t="shared" si="0"/>
-        <v>300525.92036063102</v>
+        <v>292476.55252038006</v>
       </c>
       <c r="E10" s="13">
         <f t="shared" si="1"/>
-        <v>-808267.46806912101</v>
+        <v>-822811.49228117825</v>
       </c>
       <c r="F10" s="14" t="s">
         <v>5</v>
@@ -3390,18 +3390,18 @@
       </c>
       <c r="D11" s="13">
         <f t="shared" si="0"/>
-        <v>341506.72768253525</v>
+        <v>329365.48707250005</v>
       </c>
       <c r="E11" s="13">
         <f t="shared" si="1"/>
-        <v>-466760.74038658576</v>
+        <v>-493446.00520867819</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="17">
         <f>NPV(G8,C8:C19)+C7</f>
-        <v>331969.87063950836</v>
+        <v>266545.94329153886</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3413,11 +3413,11 @@
       </c>
       <c r="D12" s="13">
         <f t="shared" si="0"/>
-        <v>403598.85998845071</v>
+        <v>385743.36323806312</v>
       </c>
       <c r="E12" s="13">
         <f t="shared" si="1"/>
-        <v>-63161.88039813505</v>
+        <v>-107702.64197061508</v>
       </c>
       <c r="F12" s="22" t="s">
         <v>9</v>
@@ -3436,11 +3436,11 @@
       </c>
       <c r="D13" s="13">
         <f t="shared" si="0"/>
-        <v>395131.75103764399</v>
+        <v>374248.58526215405</v>
       </c>
       <c r="E13" s="21">
         <f t="shared" si="1"/>
-        <v>331969.87063950894</v>
+        <v>266545.94329153898</v>
       </c>
       <c r="F13" s="26" t="s">
         <v>11</v>
@@ -3458,7 +3458,7 @@
       </c>
       <c r="E14" s="21">
         <f t="shared" si="1"/>
-        <v>331969.87063950894</v>
+        <v>266545.94329153898</v>
       </c>
       <c r="F14" s="28" t="s">
         <v>13</v>
@@ -3476,7 +3476,7 @@
       </c>
       <c r="E15" s="21">
         <f t="shared" si="1"/>
-        <v>331969.87063950894</v>
+        <v>266545.94329153898</v>
       </c>
       <c r="F15" s="28"/>
       <c r="G15" s="29"/>
@@ -3492,7 +3492,7 @@
       </c>
       <c r="E16" s="21">
         <f t="shared" si="1"/>
-        <v>331969.87063950894</v>
+        <v>266545.94329153898</v>
       </c>
       <c r="F16" s="28"/>
       <c r="G16" s="29"/>
@@ -3508,7 +3508,7 @@
       </c>
       <c r="E17" s="21">
         <f t="shared" si="1"/>
-        <v>331969.87063950894</v>
+        <v>266545.94329153898</v>
       </c>
       <c r="F17" s="28"/>
       <c r="G17" s="29"/>
@@ -3524,12 +3524,12 @@
       </c>
       <c r="E18" s="21">
         <f t="shared" si="1"/>
-        <v>331969.87063950894</v>
+        <v>266545.94329153898</v>
       </c>
       <c r="F18" s="28"/>
       <c r="G18" s="29"/>
     </row>
-    <row r="19" spans="2:7" ht="75.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" ht="110.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="10">
         <v>12</v>
       </c>
@@ -3540,7 +3540,7 @@
       </c>
       <c r="E19" s="21">
         <f t="shared" si="1"/>
-        <v>331969.87063950894</v>
+        <v>266545.94329153898</v>
       </c>
       <c r="F19" s="30"/>
       <c r="G19" s="31"/>

</xml_diff>

<commit_message>
Update Análise Financeira PROJ1.xlsx
</commit_message>
<xml_diff>
--- a/Analise Financeira/Análise Financeira PROJ1.xlsx
+++ b/Analise Financeira/Análise Financeira PROJ1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gestao-de-Portfolios\Analise Financeira\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32072C6-A334-4A72-A65A-DA9150BDD14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C22B8E6-9EAF-4796-910A-BE85255AA2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView showSheetTabs="0" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{5407E0C7-D3D1-4456-BA1C-167F3E5756A9}"/>
   </bookViews>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>VALOR PRESENTE
 ACUMULADO</t>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>Com uma Taxa Mínima de Atratividade (TMA) de 11%, o projeto continua sendo financeiramente viável. O Valor Presente Líquido (VPL) é positivo, atingindo R$ 266.545,94, o que indica que o valor presente dos fluxos de caixa futuros supera o investimento inicial de R$ 1.584.000,00. O período de payback é de aproximadamente 5,29 anos, destacando um tempo relativamente longo para recuperar o capital investido. A Taxa Interna de Retorno (TIR) de 15,68% supera a TMA de 11%, sugerindo que o projeto oferece um retorno superior ao custo de oportunidade do capital. Com um Retorno sobre o Investimento (ROI) de 77%, o projeto demonstra uma boa relação custo-benefício e reforça sua atratividade financeira. Portanto, é recomendada sua aprovação, pois o projeto oferece um retorno significativo com risco controlado.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Projeto de Pesquisa e Melhoria Contínua dos processos</t>
   </si>
 </sst>
 </file>
@@ -3230,8 +3233,8 @@
   <dimension ref="B2:G25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K19" sqref="K19"/>
+      <pane ySplit="6" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3265,7 +3268,9 @@
       <c r="B4" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="32"/>
+      <c r="C4" s="32" t="s">
+        <v>14</v>
+      </c>
       <c r="D4" s="33"/>
       <c r="E4" s="33"/>
       <c r="F4" s="33"/>

</xml_diff>